<commit_message>
created all tables in database and updated table schema
</commit_message>
<xml_diff>
--- a/documentation/Table Schema.xlsx
+++ b/documentation/Table Schema.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoaan\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\warehouse-management\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811F18CD-1999-4357-8B80-E959800BABB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A3BA8C-4856-429D-AB67-92E48E556353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B6BBB61F-5AD9-44A5-A1F1-FF8706F21B9B}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{B6BBB61F-5AD9-44A5-A1F1-FF8706F21B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FC0F6A-8FBB-44B9-9595-7B65EF3C4C8D}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1434,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8088F7C-B689-4E61-896C-3156FD66AF3F}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="A2:I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,7 +1485,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -1578,7 +1578,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1601,7 +1601,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1659,7 +1659,7 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1959,14 +1959,14 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="70.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2353,7 +2353,7 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
implement code to create tables for MS SQL System Management Studio
</commit_message>
<xml_diff>
--- a/documentation/Table Schema.xlsx
+++ b/documentation/Table Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\warehouse-management\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A3BA8C-4856-429D-AB67-92E48E556353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07141CD9-C141-4066-8F2A-163BBAA1E295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{B6BBB61F-5AD9-44A5-A1F1-FF8706F21B9B}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="8" xr2:uid="{B6BBB61F-5AD9-44A5-A1F1-FF8706F21B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -668,7 +668,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1159,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8088F7C-B689-4E61-896C-3156FD66AF3F}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -2412,8 +2412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F2133B-BC91-467B-BFB1-F58DCF4F441F}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Preliminary Procedures and Tests
</commit_message>
<xml_diff>
--- a/documentation/Table Schema.xlsx
+++ b/documentation/Table Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal Projects\warehouse-management\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07141CD9-C141-4066-8F2A-163BBAA1E295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9E745D-87CA-48E4-ACD4-C709FF63795F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="8" xr2:uid="{B6BBB61F-5AD9-44A5-A1F1-FF8706F21B9B}"/>
+    <workbookView xWindow="-22512" yWindow="648" windowWidth="21600" windowHeight="11832" xr2:uid="{B6BBB61F-5AD9-44A5-A1F1-FF8706F21B9B}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -314,6 +314,9 @@
   </si>
   <si>
     <t>tells which operation was used (INS, DEL, UPD)</t>
+  </si>
+  <si>
+    <t>binary</t>
   </si>
 </sst>
 </file>
@@ -667,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FC0F6A-8FBB-44B9-9595-7B65EF3C4C8D}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>256</v>
+        <v>50</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -772,10 +775,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="C4">
-        <v>256</v>
+        <v>64</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1159,7 +1162,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1438,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,7 +1488,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -1578,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -1601,7 +1604,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1659,7 +1662,7 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1959,14 +1962,14 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="70.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -2214,7 +2217,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" t="b">
         <v>0</v>
@@ -2353,7 +2356,7 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -2412,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F2133B-BC91-467B-BFB1-F58DCF4F441F}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>